<commit_message>
added fields to retailers, map and print work done.
</commit_message>
<xml_diff>
--- a/public/uploads/ck_retailers.xlsx
+++ b/public/uploads/ck_retailers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>retailer_code</t>
   </si>
@@ -58,10 +58,13 @@
     <t>sunil006</t>
   </si>
   <si>
-    <t>KG10</t>
+    <t>KG11</t>
   </si>
   <si>
     <t>Kesav Electronics</t>
+  </si>
+  <si>
+    <t>sunil009</t>
   </si>
 </sst>
 </file>
@@ -76,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,15 +164,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,7 +239,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>2</v>

</xml_diff>